<commit_message>
upload metadata for newly added books
</commit_message>
<xml_diff>
--- a/divinity_law/books to be linked to book chapters.xlsx
+++ b/divinity_law/books to be linked to book chapters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\vandycite\divinity_law\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baskausj/github/vandycite/divinity_law/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F87C31FE-45E8-4DB5-8871-C0FEF60F76F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04093951-C09E-634F-B219-4BC1DFEA68B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CD7E19B3-86BD-4F98-88B9-52FD63191D7A}"/>
+    <workbookView xWindow="28480" yWindow="3200" windowWidth="22080" windowHeight="11580" xr2:uid="{CD7E19B3-86BD-4F98-88B9-52FD63191D7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>title</t>
   </si>
@@ -141,13 +141,55 @@
   </si>
   <si>
     <t>https://ebookcentral.proquest.com/lib/vand/detail.action?docID=4694024</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>already in</t>
+  </si>
+  <si>
+    <t>qid</t>
+  </si>
+  <si>
+    <t>Q96243598</t>
+  </si>
+  <si>
+    <t>Q57310379</t>
+  </si>
+  <si>
+    <t>Q110920786</t>
+  </si>
+  <si>
+    <t>10.1163/9789004227163</t>
+  </si>
+  <si>
+    <t>added</t>
+  </si>
+  <si>
+    <t>Q111083718</t>
+  </si>
+  <si>
+    <t>Q111083719</t>
+  </si>
+  <si>
+    <t>Q111083720</t>
+  </si>
+  <si>
+    <t>Q111083722</t>
+  </si>
+  <si>
+    <t>Q111083723</t>
+  </si>
+  <si>
+    <t>no author or editor data, added</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,6 +232,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Liberation Sans"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -230,7 +277,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -248,6 +295,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -563,156 +612,216 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8F6D92-BCEA-4F48-8242-500FB132928E}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="41.26953125" style="4" customWidth="1"/>
-    <col min="2" max="3" width="22.6328125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="30.453125" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="4"/>
+    <col min="1" max="1" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="25.83203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="30.5" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="8.6640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:7">
+      <c r="A2" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7">
       <c r="A3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:7">
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:7" ht="32">
+      <c r="A5" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:7" ht="16">
+      <c r="A6" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7">
       <c r="A7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="F7" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:7">
+      <c r="A8" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:7" s="7" customFormat="1">
+      <c r="A9" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="E9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="10"/>
+      <c r="G9" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="7" t="s">
+    <row r="10" spans="1:7" s="8" customFormat="1" ht="16">
+      <c r="C10" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="G11" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:7" s="8" customFormat="1">
+      <c r="C12" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="G12" s="8" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E5" r:id="rId1" xr:uid="{0C5953B6-4E55-417F-ADD7-4FF156316D97}"/>
-    <hyperlink ref="D6" r:id="rId2" display="http://dx.doi.org/10.5040/9780567659644" xr:uid="{8271D427-6371-4E3F-BAE7-C1268CC6299D}"/>
-    <hyperlink ref="C10" r:id="rId3" tooltip="Search for more by this author" display="https://www.worldcat.org/search?q=au%3AAdmirand%2C+Peter%2C&amp;qt=hot_author" xr:uid="{840F7098-3803-4FE4-8904-0B5E102B85D3}"/>
-    <hyperlink ref="E11" r:id="rId4" tooltip="This link opens in a new window" xr:uid="{8510916E-21AB-4FFB-81C0-9982B311430C}"/>
+    <hyperlink ref="G5" r:id="rId1" xr:uid="{0C5953B6-4E55-417F-ADD7-4FF156316D97}"/>
+    <hyperlink ref="F6" r:id="rId2" display="http://dx.doi.org/10.5040/9780567659644" xr:uid="{8271D427-6371-4E3F-BAE7-C1268CC6299D}"/>
+    <hyperlink ref="E10" r:id="rId3" tooltip="Search for more by this author" display="https://www.worldcat.org/search?q=au%3AAdmirand%2C+Peter%2C&amp;qt=hot_author" xr:uid="{840F7098-3803-4FE4-8904-0B5E102B85D3}"/>
+    <hyperlink ref="G11" r:id="rId4" tooltip="This link opens in a new window" xr:uid="{8510916E-21AB-4FFB-81C0-9982B311430C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId5"/>

</xml_diff>

<commit_message>
Update books to be linked to book chapters.xlsx
</commit_message>
<xml_diff>
--- a/divinity_law/books to be linked to book chapters.xlsx
+++ b/divinity_law/books to be linked to book chapters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baskausj/github/vandycite/divinity_law/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04093951-C09E-634F-B219-4BC1DFEA68B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03047227-F440-024D-AF79-2B118B47469A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28480" yWindow="3200" windowWidth="22080" windowHeight="11580" xr2:uid="{CD7E19B3-86BD-4F98-88B9-52FD63191D7A}"/>
+    <workbookView xWindow="6260" yWindow="3060" windowWidth="22080" windowHeight="11580" xr2:uid="{CD7E19B3-86BD-4F98-88B9-52FD63191D7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -615,7 +615,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
append manually added monographs
</commit_message>
<xml_diff>
--- a/divinity_law/books to be linked to book chapters.xlsx
+++ b/divinity_law/books to be linked to book chapters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baskausj/github/vandycite/divinity_law/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03047227-F440-024D-AF79-2B118B47469A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB654E9D-1CCE-A049-B883-02147A820141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6260" yWindow="3060" windowWidth="22080" windowHeight="11580" xr2:uid="{CD7E19B3-86BD-4F98-88B9-52FD63191D7A}"/>
+    <workbookView xWindow="24180" yWindow="16500" windowWidth="27020" windowHeight="10780" xr2:uid="{CD7E19B3-86BD-4F98-88B9-52FD63191D7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t>title</t>
   </si>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>In the Shadow of Bezalel</t>
-  </si>
-  <si>
-    <t> Alejandro F. Botta.</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -122,9 +119,6 @@
     <t>Loss and Hope: Global, Interreligious and Interdisciplinary Perspectives</t>
   </si>
   <si>
-    <t>Peter Admirand</t>
-  </si>
-  <si>
     <t>Preaching the headlines</t>
   </si>
   <si>
@@ -137,9 +131,6 @@
     <t>Conundrums in Practical Theology</t>
   </si>
   <si>
-    <t>Joyce Ann Mercer, Bonnie J. Miller-McLemore</t>
-  </si>
-  <si>
     <t>https://ebookcentral.proquest.com/lib/vand/detail.action?docID=4694024</t>
   </si>
   <si>
@@ -183,13 +174,34 @@
   </si>
   <si>
     <t>no author or editor data, added</t>
+  </si>
+  <si>
+    <t> Alejandro F. Botta. Q55990040</t>
+  </si>
+  <si>
+    <t>Peter Admirand Q107464477</t>
+  </si>
+  <si>
+    <t>Joyce Ann Mercer Q57435308, Bonnie J. Miller-McLemore Q63038665</t>
+  </si>
+  <si>
+    <t>Q111088301</t>
+  </si>
+  <si>
+    <t>added manually with Vanderbot</t>
+  </si>
+  <si>
+    <t>Q111088304</t>
+  </si>
+  <si>
+    <t>Q111088307</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +249,12 @@
       <color theme="1"/>
       <name val="Liberation Sans"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -277,7 +295,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -297,6 +315,8 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -615,7 +635,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
@@ -631,10 +651,10 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -651,10 +671,10 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>3</v>
@@ -668,10 +688,10 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>6</v>
@@ -684,136 +704,154 @@
       </c>
     </row>
     <row r="4" spans="1:7">
+      <c r="A4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="32">
       <c r="A5" s="12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="F5" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="16">
       <c r="A6" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="F6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="9" t="s">
         <v>19</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="7" customFormat="1">
       <c r="A9" s="12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>25</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="8" customFormat="1" ht="16">
+      <c r="A10" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" s="8" customFormat="1" ht="16">
-      <c r="C10" s="7" t="s">
-        <v>27</v>
-      </c>
       <c r="E10" s="3" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="4" t="s">
+    </row>
+    <row r="12" spans="1:7" s="8" customFormat="1">
+      <c r="A12" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="E12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="13" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="8" customFormat="1">
-      <c r="C12" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -822,8 +860,9 @@
     <hyperlink ref="F6" r:id="rId2" display="http://dx.doi.org/10.5040/9780567659644" xr:uid="{8271D427-6371-4E3F-BAE7-C1268CC6299D}"/>
     <hyperlink ref="E10" r:id="rId3" tooltip="Search for more by this author" display="https://www.worldcat.org/search?q=au%3AAdmirand%2C+Peter%2C&amp;qt=hot_author" xr:uid="{840F7098-3803-4FE4-8904-0B5E102B85D3}"/>
     <hyperlink ref="G11" r:id="rId4" tooltip="This link opens in a new window" xr:uid="{8510916E-21AB-4FFB-81C0-9982B311430C}"/>
+    <hyperlink ref="G12" r:id="rId5" xr:uid="{50CFC5AE-ADAE-E04A-99D6-B8CC4A9A39A1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId5"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>